<commit_message>
Reconozco q es un mosntruo de codigo pero ya los rfc9 y rfc 10 están listos.
</commit_message>
<xml_diff>
--- a/docs/IndicesIntroducidos.xlsx
+++ b/docs/IndicesIntroducidos.xlsx
@@ -265,8 +265,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -299,11 +301,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E66" sqref="A56:E66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E50" sqref="A1:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>